<commit_message>
Proposal V1.3 dan Biaya V1.2
</commit_message>
<xml_diff>
--- a/biaya.xlsx
+++ b/biaya.xlsx
@@ -512,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -772,9 +772,10 @@
         <v>20</v>
       </c>
       <c r="E20" s="7">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="F20" s="7">
+        <f>E20*C20</f>
         <v>50000</v>
       </c>
     </row>
@@ -792,7 +793,7 @@
         <v>200000</v>
       </c>
       <c r="F21" s="7">
-        <f t="shared" ref="F20:F23" si="2">E21*C21</f>
+        <f t="shared" ref="F21:F23" si="2">E21*C21</f>
         <v>200000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Proposal V1.2 dan Biaya V1.3
</commit_message>
<xml_diff>
--- a/biaya.xlsx
+++ b/biaya.xlsx
@@ -512,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -772,9 +772,10 @@
         <v>20</v>
       </c>
       <c r="E20" s="7">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="F20" s="7">
+        <f>E20*C20</f>
         <v>50000</v>
       </c>
     </row>
@@ -792,7 +793,7 @@
         <v>200000</v>
       </c>
       <c r="F21" s="7">
-        <f t="shared" ref="F20:F23" si="2">E21*C21</f>
+        <f t="shared" ref="F21:F23" si="2">E21*C21</f>
         <v>200000</v>
       </c>
     </row>

</xml_diff>